<commit_message>
Excel indirme: oturum bazlı, bellekten oluşturma; herkese açık indirme yerine kişisel indirme
</commit_message>
<xml_diff>
--- a/data/sonuclar.xlsx
+++ b/data/sonuclar.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -744,6 +744,132 @@
         <v>34.61</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-08-11 16:49</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>gh</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>gh</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>32</v>
+      </c>
+      <c r="E6" t="n">
+        <v>31</v>
+      </c>
+      <c r="F6" t="n">
+        <v>30</v>
+      </c>
+      <c r="G6" t="n">
+        <v>27</v>
+      </c>
+      <c r="H6" t="n">
+        <v>31.5</v>
+      </c>
+      <c r="I6" t="n">
+        <v>28.5</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.3896</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.2666</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.2041</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.1396</v>
+      </c>
+      <c r="N6" t="n">
+        <v>38.96</v>
+      </c>
+      <c r="O6" t="n">
+        <v>26.66</v>
+      </c>
+      <c r="P6" t="n">
+        <v>20.41</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>13.96</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-08-11 17:06</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>yaren</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>cvf</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>39</v>
+      </c>
+      <c r="E7" t="n">
+        <v>35</v>
+      </c>
+      <c r="F7" t="n">
+        <v>28</v>
+      </c>
+      <c r="G7" t="n">
+        <v>29</v>
+      </c>
+      <c r="H7" t="n">
+        <v>37</v>
+      </c>
+      <c r="I7" t="n">
+        <v>28.5</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>%45.77</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>%31.32</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>%13.61</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>%9.31</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
AI yorum: serbest metin ve kişiye özel ton; Excel: oturumdan bellekten indirme
</commit_message>
<xml_diff>
--- a/data/sonuclar.xlsx
+++ b/data/sonuclar.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -870,6 +870,475 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-08-11 17:20</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>yaren</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>cvf</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>35</v>
+      </c>
+      <c r="E8" t="n">
+        <v>29</v>
+      </c>
+      <c r="F8" t="n">
+        <v>24</v>
+      </c>
+      <c r="G8" t="n">
+        <v>23</v>
+      </c>
+      <c r="H8" t="n">
+        <v>32</v>
+      </c>
+      <c r="I8" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>%32.64</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>%34.03</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>%16.32</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>%17.01</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-08-12 07:50</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>yaren</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>yaren</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>31</v>
+      </c>
+      <c r="E9" t="n">
+        <v>33</v>
+      </c>
+      <c r="F9" t="n">
+        <v>30</v>
+      </c>
+      <c r="G9" t="n">
+        <v>31</v>
+      </c>
+      <c r="H9" t="n">
+        <v>32</v>
+      </c>
+      <c r="I9" t="n">
+        <v>30.5</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.42</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>%42.36</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>%24.31</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>%21.18</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>%12.15</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-08-12 07:54</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>yaren</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>yaren</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>33</v>
+      </c>
+      <c r="E10" t="n">
+        <v>31</v>
+      </c>
+      <c r="F10" t="n">
+        <v>27</v>
+      </c>
+      <c r="G10" t="n">
+        <v>29</v>
+      </c>
+      <c r="H10" t="n">
+        <v>32</v>
+      </c>
+      <c r="I10" t="n">
+        <v>28</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.39</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>%38.89</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>%27.78</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>%19.44</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>%13.89</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-08-12 07:55</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>yaren</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>yaren</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>45</v>
+      </c>
+      <c r="E11" t="n">
+        <v>48</v>
+      </c>
+      <c r="F11" t="n">
+        <v>45</v>
+      </c>
+      <c r="G11" t="n">
+        <v>44</v>
+      </c>
+      <c r="H11" t="n">
+        <v>46.5</v>
+      </c>
+      <c r="I11" t="n">
+        <v>44.5</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>%89.81</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>%7.06</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>%2.9</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>%0.23</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-08-12 07:56</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>yaren</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>yaren</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>33</v>
+      </c>
+      <c r="E12" t="n">
+        <v>21</v>
+      </c>
+      <c r="F12" t="n">
+        <v>25</v>
+      </c>
+      <c r="G12" t="n">
+        <v>20</v>
+      </c>
+      <c r="H12" t="n">
+        <v>27</v>
+      </c>
+      <c r="I12" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.26</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>%26.37</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>%29.88</t>
+        </is>
+      </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>%20.51</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>%23.24</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-08-12 08:09</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>yaren</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>yaren</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>19</v>
+      </c>
+      <c r="E13" t="n">
+        <v>25</v>
+      </c>
+      <c r="F13" t="n">
+        <v>28</v>
+      </c>
+      <c r="G13" t="n">
+        <v>24</v>
+      </c>
+      <c r="H13" t="n">
+        <v>22</v>
+      </c>
+      <c r="I13" t="n">
+        <v>26</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>%24.83</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>%21.01</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>%29.34</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>%24.83</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-08-12 08:19</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>asdf</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>36</v>
+      </c>
+      <c r="E14" t="n">
+        <v>23</v>
+      </c>
+      <c r="F14" t="n">
+        <v>25</v>
+      </c>
+      <c r="G14" t="n">
+        <v>29</v>
+      </c>
+      <c r="H14" t="n">
+        <v>29.5</v>
+      </c>
+      <c r="I14" t="n">
+        <v>27</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>%34.57</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>%26.89</t>
+        </is>
+      </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>%21.68</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>%16.86</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Yeni revize: yapay zeka yorum çeşitliliği artırıldı
</commit_message>
<xml_diff>
--- a/data/sonuclar.xlsx
+++ b/data/sonuclar.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2350,8 +2350,6 @@
           <t>2025-08-12 14:21</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr"/>
-      <c r="C30" t="inlineStr"/>
       <c r="D30" t="n">
         <v>48</v>
       </c>
@@ -2400,6 +2398,140 @@
       <c r="Q30" t="inlineStr">
         <is>
           <t>%14.06</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-08-15 11:57</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Hacer Yaren Ünsal</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Hacer Yaren Ünsal</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>44</v>
+      </c>
+      <c r="E31" t="n">
+        <v>33</v>
+      </c>
+      <c r="F31" t="n">
+        <v>31</v>
+      </c>
+      <c r="G31" t="n">
+        <v>26</v>
+      </c>
+      <c r="H31" t="n">
+        <v>38.5</v>
+      </c>
+      <c r="I31" t="n">
+        <v>28.5</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="L31" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>%47.62</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>%32.58</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>%11.75</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>%8.04</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-08-18 09:55</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Hacer Yaren Ünsal</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Hacer Yaren Ünsal</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>36</v>
+      </c>
+      <c r="E32" t="n">
+        <v>31</v>
+      </c>
+      <c r="F32" t="n">
+        <v>26</v>
+      </c>
+      <c r="G32" t="n">
+        <v>31</v>
+      </c>
+      <c r="H32" t="n">
+        <v>33.5</v>
+      </c>
+      <c r="I32" t="n">
+        <v>28.5</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="L32" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>%41.44</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>%28.35</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>%17.94</t>
+        </is>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>%12.27</t>
         </is>
       </c>
     </row>

</xml_diff>